<commit_message>
model and template with unit, description and enum
</commit_message>
<xml_diff>
--- a/template_pegase_v1/behavior.xlsx
+++ b/template_pegase_v1/behavior.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Operator</t>
   </si>
@@ -39,6 +39,27 @@
   </si>
   <si>
     <t>#date</t>
+  </si>
+  <si>
+    <t>#Manipulateur</t>
+  </si>
+  <si>
+    <t>#Desc:IdentifiantEchantillon</t>
+  </si>
+  <si>
+    <t>#Date</t>
+  </si>
+  <si>
+    <t>#ModeOderatoireLaboratoire</t>
+  </si>
+  <si>
+    <t>#AppareilLogicielCritique</t>
+  </si>
+  <si>
+    <t>#ProduitCritique</t>
+  </si>
+  <si>
+    <t>#LieuStockageDonneesBrutes</t>
   </si>
 </sst>
 </file>
@@ -83,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -135,6 +156,29 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>